<commit_message>
Adding Lecture 10 sample code
</commit_message>
<xml_diff>
--- a/A3/Assignment 3 Check Tool.xlsx
+++ b/A3/Assignment 3 Check Tool.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rbenitez\source\repos\COP3014\A3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{89AD82D5-6E56-403E-96B0-9BC90AE73F42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4067C325-3AE5-4A31-B4CD-7832B83CEFFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="384" windowWidth="23256" windowHeight="12576" xr2:uid="{7B1CC5FD-D9F9-4D4E-A5DD-EEF3426B2857}"/>
+    <workbookView xWindow="12" yWindow="12" windowWidth="23016" windowHeight="12336" xr2:uid="{7B1CC5FD-D9F9-4D4E-A5DD-EEF3426B2857}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>STD</t>
   </si>
@@ -48,12 +48,124 @@
   <si>
     <t>n</t>
   </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>C/B</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Amplitude</t>
+  </si>
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t>Related to Period</t>
+  </si>
+  <si>
+    <t>H-Shift</t>
+  </si>
+  <si>
+    <t>V-Shift</t>
+  </si>
+  <si>
+    <t>Related to H-Shift</t>
+  </si>
+  <si>
+    <t>Computed</t>
+  </si>
+  <si>
+    <t>Enter</t>
+  </si>
+  <si>
+    <t>Y=1.5 * sin(2*pi/8 * (x + 1)) + 0</t>
+  </si>
+  <si>
+    <t>rn</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>% oper</t>
+  </si>
+  <si>
+    <t>Q x %oper</t>
+  </si>
+  <si>
+    <t>Checkpoint</t>
+  </si>
+  <si>
+    <t>Xronos</t>
+  </si>
+  <si>
+    <t>Midterm</t>
+  </si>
+  <si>
+    <t>final</t>
+  </si>
+  <si>
+    <t>Bonus</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>% Tot</t>
+  </si>
+  <si>
+    <t>% ea</t>
+  </si>
+  <si>
+    <t>Est</t>
+  </si>
+  <si>
+    <t>r1</t>
+  </si>
+  <si>
+    <t>r2</t>
+  </si>
+  <si>
+    <t>c1</t>
+  </si>
+  <si>
+    <t>c2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,12 +182,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -87,21 +205,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -114,6 +249,1681 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$K$8:$K$138</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="131"/>
+                <c:pt idx="0">
+                  <c:v>-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-2.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-2.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-2.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-2.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-2.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-1.9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-1.8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-1.7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-1.6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-1.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-1.4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-1.3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-1.2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-0.9</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-0.8</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-0.7</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-0.6</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-0.4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-0.3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-0.2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-0.1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2.5000000000000102</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2.9000000000000101</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>3.0000000000000102</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>3.2000000000000099</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>3.30000000000001</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>3.4000000000000101</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>3.5000000000000102</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>3.6000000000000099</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>3.7000000000000099</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>3.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>3.9000000000000101</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>4.0000000000000098</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>4.1000000000000103</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>4.2000000000000099</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>4.3000000000000096</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>4.4000000000000101</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>4.5000000000000098</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>4.6000000000000103</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>4.7000000000000099</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>4.8000000000000096</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>4.9000000000000101</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>5.0000000000000098</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>5.1000000000000103</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>5.2000000000000099</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>5.3000000000000096</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>5.4000000000000101</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>5.5000000000000098</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>5.6000000000000103</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>5.7000000000000099</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>5.8000000000000096</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>5.9000000000000101</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>6.0000000000000098</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>6.1000000000000103</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>6.2000000000000099</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>6.3000000000000096</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>6.4000000000000101</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>6.5000000000000098</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>6.6000000000000103</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>6.7000000000000099</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>6.8000000000000096</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>6.9000000000000101</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>7.1</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>7.3</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>7.7</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>7.8</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>7.9</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>8.1</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>8.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>8.4</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>8.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>8.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>8.9</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>9.1</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>9.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>9.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>9.6</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>9.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>9.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>9.9</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$8:$L$138</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="131"/>
+                <c:pt idx="0">
+                  <c:v>4.90059381963448E-16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.61803398874989524</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1755705045849467</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.6180339887498951</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9021130325903073</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.9021130325903071</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.6180339887498936</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1755705045849474</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.61803398874989457</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-2.45029690981724E-16</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.61803398874989501</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-1.1755705045849465</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-1.6180339887498949</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-1.9021130325903073</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-1.9021130325903071</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-1.6180339887498949</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-1.1755705045849463</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-0.61803398874989568</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.61803398874989479</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.1755705045849463</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.6180339887498949</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.9021130325903071</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.9021130325903073</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.6180339887498949</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.1755705045849465</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.61803398874989501</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.45029690981724E-16</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-0.61803398874989457</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-1.1755705045849461</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-1.6180339887498947</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-1.9021130325903071</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-1.9021130325903073</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-1.6180339887498951</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-1.1755705045849467</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-0.61803398874989524</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-4.90059381963448E-16</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.61803398874989435</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.1755705045849458</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.6180339887498945</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.9021130325903071</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.9021130325903073</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.6180339887498953</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.1755705045849467</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.61803398874989557</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>7.3508907294517201E-16</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-0.61803398874989413</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>-1.1755705045849456</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-1.6180339887498922</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>-1.9021130325903068</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>-1.9021130325903075</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>-1.6180339887498953</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-1.1755705045848952</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-0.61803398874983495</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>6.2968727454482121E-14</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.6180339887498939</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.1755705045849971</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.6180339887499318</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.9021130325903266</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1.9021130325902889</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.618033988749858</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.1755705045848954</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.61803398874983517</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>-5.9170984084699896E-14</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>-0.61803398874995785</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>-1.1755705045849969</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>-1.6180339887499295</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>-1.9021130325903266</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>-1.9021130325902877</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>-1.6180339887498603</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>-1.1755705045848956</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>-0.61803398874983206</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>5.5373240714917671E-14</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.61803398874995763</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1.1755705045849967</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1.6180339887499295</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1.9021130325903264</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1.902113032590288</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1.6180339887498603</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1.1755705045849016</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.61803398874983906</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>-6.2233638381536949E-14</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>-0.61803398874995741</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>-1.1755705045849965</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>-1.6180339887499293</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>-1.9021130325903264</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>-1.902113032590288</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>-1.6180339887498605</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>-1.1755705045849019</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>-0.61803398874983928</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>-1.960237527853792E-15</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.61803398874988957</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>1.1755705045849447</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>1.6180339887498916</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>1.9021130325903066</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>1.9021130325903077</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>1.618033988749894</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>1.1755705045849481</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>0.61803398874989357</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>2.205267218835516E-15</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>-0.61803398874988935</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>-1.1755705045849387</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>-1.6180339887498956</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>-1.9021130325903064</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>-1.902113032590308</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>-1.6180339887498982</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>-1.1755705045849425</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>-0.61803398874989379</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>-2.45029690981724E-15</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>0.61803398874988913</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>1.1755705045849385</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>1.6180339887498913</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>1.9021130325903064</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>1.9021130325903057</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>1.6180339887498985</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>1.1755705045849369</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>0.61803398874989401</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>9.8007539583999659E-15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7522-4597-BFB0-F5363BDF67ED}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1782527904"/>
+        <c:axId val="1782527488"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1782527904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1782527488"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1782527488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1782527904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1EEDB84D-C0E6-ABBD-8571-C13F269F1799}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -413,10 +2223,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A969B68F-7DCA-4A8E-B2B2-0C73FEEC8797}">
-  <dimension ref="A1:E1000"/>
+  <dimension ref="A1:Y1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -424,7 +2234,7 @@
     <col min="1" max="2" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -439,7 +2249,7 @@
         <v>501.42</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>339</v>
       </c>
@@ -455,7 +2265,7 @@
         <v>298.84665566139432</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>556</v>
       </c>
@@ -464,7 +2274,7 @@
         <v>2978.9763999999982</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>723</v>
       </c>
@@ -473,7 +2283,7 @@
         <v>49097.696399999993</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>83</v>
       </c>
@@ -481,8 +2291,20 @@
         <f>(A5-$E$1)^2</f>
         <v>175075.29640000002</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>28</v>
       </c>
@@ -490,8 +2312,9 @@
         <f>(A6-$E$1)^2</f>
         <v>224126.4964</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>304</v>
       </c>
@@ -499,8 +2322,26 @@
         <f>(A7-$E$1)^2</f>
         <v>38974.656400000007</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="5">
+        <v>2</v>
+      </c>
+      <c r="I7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>721</v>
       </c>
@@ -508,8 +2349,28 @@
         <f>(A8-$E$1)^2</f>
         <v>48215.376399999994</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="5">
+        <f>2*PI()/H5</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="I8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" s="1">
+        <v>-3</v>
+      </c>
+      <c r="L8" s="6">
+        <f>$H$7*SIN(($H$8*K8)-$H$9)+$H$11</f>
+        <v>4.90059381963448E-16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>583</v>
       </c>
@@ -517,8 +2378,28 @@
         <f>(A9-$E$1)^2</f>
         <v>6655.2963999999974</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="5">
+        <f>H10*H8</f>
+        <v>-3.1415926535897931</v>
+      </c>
+      <c r="I9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" s="1">
+        <v>-2.9</v>
+      </c>
+      <c r="L9" s="6">
+        <f t="shared" ref="L9:L72" si="0">$H$7*SIN(($H$8*K9)-$H$9)+$H$11</f>
+        <v>0.61803398874989524</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>198</v>
       </c>
@@ -526,8 +2407,27 @@
         <f>(A10-$E$1)^2</f>
         <v>92063.696400000015</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="5">
+        <v>-1</v>
+      </c>
+      <c r="I10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="1">
+        <v>-2.8</v>
+      </c>
+      <c r="L10" s="6">
+        <f t="shared" si="0"/>
+        <v>1.1755705045849467</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>235</v>
       </c>
@@ -535,8 +2435,27 @@
         <f>(A11-$E$1)^2</f>
         <v>70979.616400000014</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" s="1">
+        <v>-2.7</v>
+      </c>
+      <c r="L11" s="6">
+        <f t="shared" si="0"/>
+        <v>1.6180339887498951</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>329</v>
       </c>
@@ -544,8 +2463,15 @@
         <f>(A12-$E$1)^2</f>
         <v>29728.656400000007</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="K12" s="1">
+        <v>-2.6</v>
+      </c>
+      <c r="L12" s="6">
+        <f t="shared" si="0"/>
+        <v>1.9021130325903073</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>877</v>
       </c>
@@ -553,8 +2479,18 @@
         <f>(A13-$E$1)^2</f>
         <v>141060.3364</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="1">
+        <v>-2.5</v>
+      </c>
+      <c r="L13" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>873</v>
       </c>
@@ -562,8 +2498,15 @@
         <f>(A14-$E$1)^2</f>
         <v>138071.69639999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="K14" s="1">
+        <v>-2.4</v>
+      </c>
+      <c r="L14" s="6">
+        <f t="shared" si="0"/>
+        <v>1.9021130325903071</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>963</v>
       </c>
@@ -571,8 +2514,15 @@
         <f>(A15-$E$1)^2</f>
         <v>213056.09639999998</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="K15" s="1">
+        <v>-2.2999999999999998</v>
+      </c>
+      <c r="L15" s="6">
+        <f t="shared" si="0"/>
+        <v>1.6180339887498936</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>630</v>
       </c>
@@ -580,8 +2530,15 @@
         <f>(A16-$E$1)^2</f>
         <v>16532.816399999996</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="K16" s="1">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="L16" s="6">
+        <f t="shared" si="0"/>
+        <v>1.1755705045849474</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>908</v>
       </c>
@@ -589,8 +2546,15 @@
         <f>(A17-$E$1)^2</f>
         <v>165307.29639999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="K17" s="1">
+        <v>-2.1</v>
+      </c>
+      <c r="L17" s="6">
+        <f t="shared" si="0"/>
+        <v>0.61803398874989457</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>103</v>
       </c>
@@ -598,8 +2562,30 @@
         <f>(A18-$E$1)^2</f>
         <v>158738.4964</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18" s="1">
+        <v>-2</v>
+      </c>
+      <c r="L18" s="6">
+        <f t="shared" si="0"/>
+        <v>-2.45029690981724E-16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>385</v>
       </c>
@@ -607,8 +2593,33 @@
         <f>(A19-$E$1)^2</f>
         <v>13553.616400000004</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D19">
+        <v>1753</v>
+      </c>
+      <c r="E19" s="1">
+        <v>10</v>
+      </c>
+      <c r="F19">
+        <f>ROUNDDOWN($D$19/E19,0)</f>
+        <v>175</v>
+      </c>
+      <c r="G19">
+        <f>F19*E19</f>
+        <v>1750</v>
+      </c>
+      <c r="H19">
+        <f>$D$19-F19*E19</f>
+        <v>3</v>
+      </c>
+      <c r="K19" s="1">
+        <v>-1.9</v>
+      </c>
+      <c r="L19" s="6">
+        <f t="shared" si="0"/>
+        <v>-0.61803398874989501</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>481</v>
       </c>
@@ -616,8 +2627,30 @@
         <f>(A20-$E$1)^2</f>
         <v>416.97640000000064</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E20" s="1">
+        <v>20</v>
+      </c>
+      <c r="F20">
+        <f>ROUNDDOWN($D$19/E20,0)</f>
+        <v>87</v>
+      </c>
+      <c r="G20">
+        <f t="shared" ref="G20:G40" si="1">F20*E20</f>
+        <v>1740</v>
+      </c>
+      <c r="H20">
+        <f>$D$19-F20*E20</f>
+        <v>13</v>
+      </c>
+      <c r="K20" s="1">
+        <v>-1.8</v>
+      </c>
+      <c r="L20" s="6">
+        <f t="shared" si="0"/>
+        <v>-1.1755705045849465</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>21</v>
       </c>
@@ -625,8 +2658,30 @@
         <f>(A21-$E$1)^2</f>
         <v>230803.37640000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E21" s="1">
+        <v>30</v>
+      </c>
+      <c r="F21">
+        <f>ROUNDDOWN($D$19/E21,0)</f>
+        <v>58</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>1740</v>
+      </c>
+      <c r="H21">
+        <f>$D$19-F21*E21</f>
+        <v>13</v>
+      </c>
+      <c r="K21" s="1">
+        <v>-1.7</v>
+      </c>
+      <c r="L21" s="6">
+        <f t="shared" si="0"/>
+        <v>-1.6180339887498949</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>963</v>
       </c>
@@ -634,8 +2689,30 @@
         <f>(A22-$E$1)^2</f>
         <v>213056.09639999998</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E22" s="1">
+        <v>40</v>
+      </c>
+      <c r="F22">
+        <f>ROUNDDOWN($D$19/E22,0)</f>
+        <v>43</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>1720</v>
+      </c>
+      <c r="H22">
+        <f>$D$19-F22*E22</f>
+        <v>33</v>
+      </c>
+      <c r="K22" s="1">
+        <v>-1.6</v>
+      </c>
+      <c r="L22" s="6">
+        <f t="shared" si="0"/>
+        <v>-1.9021130325903073</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>97</v>
       </c>
@@ -643,8 +2720,30 @@
         <f>(A23-$E$1)^2</f>
         <v>163555.53640000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E23" s="1">
+        <v>50</v>
+      </c>
+      <c r="F23">
+        <f>ROUNDDOWN($D$19/E23,0)</f>
+        <v>35</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>1750</v>
+      </c>
+      <c r="H23">
+        <f>$D$19-F23*E23</f>
+        <v>3</v>
+      </c>
+      <c r="K23" s="1">
+        <v>-1.5</v>
+      </c>
+      <c r="L23" s="6">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>415</v>
       </c>
@@ -652,8 +2751,30 @@
         <f>(A24-$E$1)^2</f>
         <v>7468.4164000000028</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E24" s="1">
+        <v>60</v>
+      </c>
+      <c r="F24">
+        <f>ROUNDDOWN($D$19/E24,0)</f>
+        <v>29</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>1740</v>
+      </c>
+      <c r="H24">
+        <f>$D$19-F24*E24</f>
+        <v>13</v>
+      </c>
+      <c r="K24" s="1">
+        <v>-1.4</v>
+      </c>
+      <c r="L24" s="6">
+        <f t="shared" si="0"/>
+        <v>-1.9021130325903071</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>563</v>
       </c>
@@ -661,8 +2782,30 @@
         <f>(A25-$E$1)^2</f>
         <v>3792.0963999999981</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E25" s="1">
+        <v>70</v>
+      </c>
+      <c r="F25">
+        <f>ROUNDDOWN($D$19/E25,0)</f>
+        <v>25</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>1750</v>
+      </c>
+      <c r="H25">
+        <f>$D$19-F25*E25</f>
+        <v>3</v>
+      </c>
+      <c r="K25" s="1">
+        <v>-1.3</v>
+      </c>
+      <c r="L25" s="6">
+        <f t="shared" si="0"/>
+        <v>-1.6180339887498949</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>86</v>
       </c>
@@ -670,8 +2813,30 @@
         <f>(A26-$E$1)^2</f>
         <v>172573.7764</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E26" s="1">
+        <v>80</v>
+      </c>
+      <c r="F26">
+        <f>ROUNDDOWN($D$19/E26,0)</f>
+        <v>21</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>1680</v>
+      </c>
+      <c r="H26">
+        <f>$D$19-F26*E26</f>
+        <v>73</v>
+      </c>
+      <c r="K26" s="1">
+        <v>-1.2</v>
+      </c>
+      <c r="L26" s="6">
+        <f t="shared" si="0"/>
+        <v>-1.1755705045849463</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>795</v>
       </c>
@@ -679,8 +2844,30 @@
         <f>(A27-$E$1)^2</f>
         <v>86189.21639999999</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E27" s="1">
+        <v>90</v>
+      </c>
+      <c r="F27">
+        <f>ROUNDDOWN($D$19/E27,0)</f>
+        <v>19</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>1710</v>
+      </c>
+      <c r="H27">
+        <f>$D$19-F27*E27</f>
+        <v>43</v>
+      </c>
+      <c r="K27" s="1">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="L27" s="6">
+        <f t="shared" si="0"/>
+        <v>-0.61803398874989568</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>6</v>
       </c>
@@ -688,8 +2875,30 @@
         <f>(A28-$E$1)^2</f>
         <v>245440.97640000001</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E28" s="1">
+        <v>100</v>
+      </c>
+      <c r="F28">
+        <f>ROUNDDOWN($D$19/E28,0)</f>
+        <v>17</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>1700</v>
+      </c>
+      <c r="H28">
+        <f>$D$19-F28*E28</f>
+        <v>53</v>
+      </c>
+      <c r="K28" s="1">
+        <v>-1</v>
+      </c>
+      <c r="L28" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>73</v>
       </c>
@@ -697,8 +2906,30 @@
         <f>(A29-$E$1)^2</f>
         <v>183543.69640000002</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E29" s="1">
+        <v>110</v>
+      </c>
+      <c r="F29">
+        <f>ROUNDDOWN($D$19/E29,0)</f>
+        <v>15</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>1650</v>
+      </c>
+      <c r="H29">
+        <f>$D$19-F29*E29</f>
+        <v>103</v>
+      </c>
+      <c r="K29" s="1">
+        <v>-0.9</v>
+      </c>
+      <c r="L29" s="6">
+        <f t="shared" si="0"/>
+        <v>0.61803398874989479</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>875</v>
       </c>
@@ -706,8 +2937,36 @@
         <f>(A30-$E$1)^2</f>
         <v>139562.01639999999</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E30" s="1">
+        <v>120</v>
+      </c>
+      <c r="F30">
+        <f>ROUNDDOWN($D$19/E30,0)</f>
+        <v>14</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>1680</v>
+      </c>
+      <c r="H30">
+        <f>$D$19-F30*E30</f>
+        <v>73</v>
+      </c>
+      <c r="K30" s="1">
+        <v>-0.8</v>
+      </c>
+      <c r="L30" s="6">
+        <f t="shared" si="0"/>
+        <v>1.1755705045849463</v>
+      </c>
+      <c r="V30" t="s">
+        <v>35</v>
+      </c>
+      <c r="W30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>299</v>
       </c>
@@ -715,8 +2974,36 @@
         <f>(A31-$E$1)^2</f>
         <v>40973.856400000004</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E31" s="1">
+        <v>130</v>
+      </c>
+      <c r="F31">
+        <f>ROUNDDOWN($D$19/E31,0)</f>
+        <v>13</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="1"/>
+        <v>1690</v>
+      </c>
+      <c r="H31">
+        <f>$D$19-F31*E31</f>
+        <v>63</v>
+      </c>
+      <c r="K31" s="1">
+        <v>-0.7</v>
+      </c>
+      <c r="L31" s="6">
+        <f t="shared" si="0"/>
+        <v>1.6180339887498949</v>
+      </c>
+      <c r="V31" t="s">
+        <v>36</v>
+      </c>
+      <c r="W31">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>960</v>
       </c>
@@ -724,8 +3011,49 @@
         <f>(A32-$E$1)^2</f>
         <v>210295.6164</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E32" s="1">
+        <v>140</v>
+      </c>
+      <c r="F32">
+        <f>ROUNDDOWN($D$19/E32,0)</f>
+        <v>12</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="1"/>
+        <v>1680</v>
+      </c>
+      <c r="H32">
+        <f>$D$19-F32*E32</f>
+        <v>73</v>
+      </c>
+      <c r="K32" s="1">
+        <v>-0.6</v>
+      </c>
+      <c r="L32" s="6">
+        <f t="shared" si="0"/>
+        <v>1.9021130325903071</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>31</v>
+      </c>
+      <c r="R32" t="s">
+        <v>33</v>
+      </c>
+      <c r="S32" t="s">
+        <v>32</v>
+      </c>
+      <c r="U32" t="s">
+        <v>34</v>
+      </c>
+      <c r="V32" t="s">
+        <v>37</v>
+      </c>
+      <c r="W32">
+        <f>2*PI()*W30</f>
+        <v>12.566370614359172</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>758</v>
       </c>
@@ -733,8 +3061,50 @@
         <f>(A33-$E$1)^2</f>
         <v>65833.296399999992</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E33" s="1">
+        <v>150</v>
+      </c>
+      <c r="F33">
+        <f>ROUNDDOWN($D$19/E33,0)</f>
+        <v>11</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="1"/>
+        <v>1650</v>
+      </c>
+      <c r="H33">
+        <f>$D$19-F33*E33</f>
+        <v>103</v>
+      </c>
+      <c r="K33" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="L33" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="P33" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q33">
+        <v>13</v>
+      </c>
+      <c r="R33" s="10">
+        <f>S33/Q33</f>
+        <v>6.9230769230769224E-3</v>
+      </c>
+      <c r="S33" s="9">
+        <v>0.09</v>
+      </c>
+      <c r="V33" t="s">
+        <v>38</v>
+      </c>
+      <c r="W33">
+        <f>2*PI()*W31</f>
+        <v>50.26548245743669</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>172</v>
       </c>
@@ -742,8 +3112,43 @@
         <f>(A34-$E$1)^2</f>
         <v>108517.53640000001</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E34" s="1">
+        <v>160</v>
+      </c>
+      <c r="F34">
+        <f>ROUNDDOWN($D$19/E34,0)</f>
+        <v>10</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="1"/>
+        <v>1600</v>
+      </c>
+      <c r="H34">
+        <f>$D$19-F34*E34</f>
+        <v>153</v>
+      </c>
+      <c r="K34" s="1">
+        <v>-0.4</v>
+      </c>
+      <c r="L34" s="6">
+        <f t="shared" si="0"/>
+        <v>1.9021130325903073</v>
+      </c>
+      <c r="P34" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q34">
+        <v>14</v>
+      </c>
+      <c r="R34" s="10">
+        <f t="shared" ref="R34:R37" si="2">S34/Q34</f>
+        <v>0.02</v>
+      </c>
+      <c r="S34" s="9">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>222</v>
       </c>
@@ -751,8 +3156,47 @@
         <f>(A35-$E$1)^2</f>
         <v>78075.536400000012</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E35" s="1">
+        <v>170</v>
+      </c>
+      <c r="F35">
+        <f>ROUNDDOWN($D$19/E35,0)</f>
+        <v>10</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="1"/>
+        <v>1700</v>
+      </c>
+      <c r="H35">
+        <f>$D$19-F35*E35</f>
+        <v>53</v>
+      </c>
+      <c r="K35" s="1">
+        <v>-0.3</v>
+      </c>
+      <c r="L35" s="6">
+        <f t="shared" si="0"/>
+        <v>1.6180339887498949</v>
+      </c>
+      <c r="P35" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q35">
+        <v>3</v>
+      </c>
+      <c r="R35" s="10">
+        <f t="shared" si="2"/>
+        <v>0.15</v>
+      </c>
+      <c r="S35" s="9">
+        <v>0.45</v>
+      </c>
+      <c r="W35">
+        <f>W32/W33</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>838</v>
       </c>
@@ -760,8 +3204,47 @@
         <f>(A36-$E$1)^2</f>
         <v>113286.09639999999</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E36" s="1">
+        <v>180</v>
+      </c>
+      <c r="F36">
+        <f>ROUNDDOWN($D$19/E36,0)</f>
+        <v>9</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="1"/>
+        <v>1620</v>
+      </c>
+      <c r="H36">
+        <f>$D$19-F36*E36</f>
+        <v>133</v>
+      </c>
+      <c r="K36" s="1">
+        <v>-0.2</v>
+      </c>
+      <c r="L36" s="6">
+        <f t="shared" si="0"/>
+        <v>1.1755705045849465</v>
+      </c>
+      <c r="P36" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q36">
+        <v>1</v>
+      </c>
+      <c r="R36" s="10">
+        <f t="shared" si="2"/>
+        <v>0.18</v>
+      </c>
+      <c r="S36" s="9">
+        <v>0.18</v>
+      </c>
+      <c r="Y36">
+        <f>2/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>759</v>
       </c>
@@ -769,8 +3252,43 @@
         <f>(A37-$E$1)^2</f>
         <v>66347.456399999995</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E37" s="1">
+        <v>190</v>
+      </c>
+      <c r="F37">
+        <f>ROUNDDOWN($D$19/E37,0)</f>
+        <v>9</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="1"/>
+        <v>1710</v>
+      </c>
+      <c r="H37">
+        <f>$D$19-F37*E37</f>
+        <v>43</v>
+      </c>
+      <c r="K37" s="1">
+        <v>-0.1</v>
+      </c>
+      <c r="L37" s="6">
+        <f t="shared" si="0"/>
+        <v>0.61803398874989501</v>
+      </c>
+      <c r="P37" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q37">
+        <v>13</v>
+      </c>
+      <c r="R37" s="10">
+        <f t="shared" si="2"/>
+        <v>1.5384615384615385E-3</v>
+      </c>
+      <c r="S37" s="9">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>475</v>
       </c>
@@ -778,8 +3296,30 @@
         <f>(A38-$E$1)^2</f>
         <v>698.01640000000089</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E38" s="1">
+        <v>200</v>
+      </c>
+      <c r="F38">
+        <f>ROUNDDOWN($D$19/E38,0)</f>
+        <v>8</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="1"/>
+        <v>1600</v>
+      </c>
+      <c r="H38">
+        <f>$D$19-F38*E38</f>
+        <v>153</v>
+      </c>
+      <c r="K38" s="1">
+        <v>0</v>
+      </c>
+      <c r="L38" s="6">
+        <f t="shared" si="0"/>
+        <v>2.45029690981724E-16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>686</v>
       </c>
@@ -787,8 +3327,30 @@
         <f>(A39-$E$1)^2</f>
         <v>34069.776399999995</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E39" s="1">
+        <v>210</v>
+      </c>
+      <c r="F39">
+        <f>ROUNDDOWN($D$19/E39,0)</f>
+        <v>8</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="1"/>
+        <v>1680</v>
+      </c>
+      <c r="H39">
+        <f>$D$19-F39*E39</f>
+        <v>73</v>
+      </c>
+      <c r="K39" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="L39" s="6">
+        <f t="shared" si="0"/>
+        <v>-0.61803398874989457</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>521</v>
       </c>
@@ -796,8 +3358,30 @@
         <f>(A40-$E$1)^2</f>
         <v>383.37639999999936</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E40" s="1">
+        <v>220</v>
+      </c>
+      <c r="F40">
+        <f>ROUNDDOWN($D$19/E40,0)</f>
+        <v>7</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="1"/>
+        <v>1540</v>
+      </c>
+      <c r="H40">
+        <f>$D$19-F40*E40</f>
+        <v>213</v>
+      </c>
+      <c r="K40" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="L40" s="6">
+        <f t="shared" si="0"/>
+        <v>-1.1755705045849461</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>756</v>
       </c>
@@ -805,8 +3389,15 @@
         <f>(A41-$E$1)^2</f>
         <v>64810.976399999992</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="K41" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="L41" s="6">
+        <f t="shared" si="0"/>
+        <v>-1.6180339887498947</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>693</v>
       </c>
@@ -814,8 +3405,15 @@
         <f>(A42-$E$1)^2</f>
         <v>36702.896399999991</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="K42" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="L42" s="6">
+        <f t="shared" si="0"/>
+        <v>-1.9021130325903071</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>967</v>
       </c>
@@ -823,8 +3421,15 @@
         <f>(A43-$E$1)^2</f>
         <v>216764.73639999999</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="K43" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L43" s="6">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>765</v>
       </c>
@@ -832,8 +3437,15 @@
         <f>(A44-$E$1)^2</f>
         <v>69474.416399999987</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="K44" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="L44" s="6">
+        <f t="shared" si="0"/>
+        <v>-1.9021130325903073</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>254</v>
       </c>
@@ -841,8 +3453,15 @@
         <f>(A45-$E$1)^2</f>
         <v>61216.656400000007</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="K45" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="L45" s="6">
+        <f t="shared" si="0"/>
+        <v>-1.6180339887498951</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>220</v>
       </c>
@@ -850,8 +3469,15 @@
         <f>(A46-$E$1)^2</f>
         <v>79197.216400000005</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="K46" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="L46" s="6">
+        <f t="shared" si="0"/>
+        <v>-1.1755705045849467</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>475</v>
       </c>
@@ -859,8 +3485,15 @@
         <f>(A47-$E$1)^2</f>
         <v>698.01640000000089</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="K47" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="L47" s="6">
+        <f t="shared" si="0"/>
+        <v>-0.61803398874989524</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>680</v>
       </c>
@@ -868,8 +3501,15 @@
         <f>(A48-$E$1)^2</f>
         <v>31890.816399999996</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="K48" s="1">
+        <v>1</v>
+      </c>
+      <c r="L48" s="6">
+        <f t="shared" si="0"/>
+        <v>-4.90059381963448E-16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>174</v>
       </c>
@@ -877,8 +3517,15 @@
         <f>(A49-$E$1)^2</f>
         <v>107203.8564</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="K49" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="L49" s="6">
+        <f t="shared" si="0"/>
+        <v>0.61803398874989435</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>645</v>
       </c>
@@ -886,8 +3533,15 @@
         <f>(A50-$E$1)^2</f>
         <v>20615.216399999994</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="K50" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="L50" s="6">
+        <f t="shared" si="0"/>
+        <v>1.1755705045849458</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>539</v>
       </c>
@@ -895,560 +3549,1176 @@
         <f>(A51-$E$1)^2</f>
         <v>1412.2563999999988</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="K51" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="L51" s="6">
+        <f t="shared" si="0"/>
+        <v>1.6180339887498945</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B52" s="1">
         <f>(A52-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="K52" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="L52" s="6">
+        <f t="shared" si="0"/>
+        <v>1.9021130325903071</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B53" s="1">
         <f>(A53-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="K53" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="L53" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B54" s="1">
         <f>(A54-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="K54" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="L54" s="6">
+        <f t="shared" si="0"/>
+        <v>1.9021130325903073</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B55" s="1">
         <f>(A55-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="K55" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="L55" s="6">
+        <f t="shared" si="0"/>
+        <v>1.6180339887498953</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B56" s="1">
         <f>(A56-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="K56" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="L56" s="6">
+        <f t="shared" si="0"/>
+        <v>1.1755705045849467</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B57" s="1">
         <f>(A57-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="K57" s="1">
+        <v>1.9</v>
+      </c>
+      <c r="L57" s="6">
+        <f t="shared" si="0"/>
+        <v>0.61803398874989557</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B58" s="1">
         <f>(A58-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="K58" s="1">
+        <v>2</v>
+      </c>
+      <c r="L58" s="6">
+        <f t="shared" si="0"/>
+        <v>7.3508907294517201E-16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B59" s="1">
         <f>(A59-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="K59" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="L59" s="6">
+        <f t="shared" si="0"/>
+        <v>-0.61803398874989413</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B60" s="1">
         <f>(A60-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="K60" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="L60" s="6">
+        <f t="shared" si="0"/>
+        <v>-1.1755705045849456</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B61" s="1">
         <f>(A61-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="K61" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="L61" s="6">
+        <f t="shared" si="0"/>
+        <v>-1.6180339887498922</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B62" s="1">
         <f>(A62-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="K62" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="L62" s="6">
+        <f t="shared" si="0"/>
+        <v>-1.9021130325903068</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B63" s="1">
         <f>(A63-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="K63" s="1">
+        <v>2.5000000000000102</v>
+      </c>
+      <c r="L63" s="6">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B64" s="1">
         <f>(A64-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K64" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="L64" s="6">
+        <f t="shared" si="0"/>
+        <v>-1.9021130325903075</v>
+      </c>
+    </row>
+    <row r="65" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B65" s="1">
         <f>(A65-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K65" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="L65" s="6">
+        <f t="shared" si="0"/>
+        <v>-1.6180339887498953</v>
+      </c>
+    </row>
+    <row r="66" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B66" s="1">
         <f>(A66-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K66" s="1">
+        <v>2.80000000000001</v>
+      </c>
+      <c r="L66" s="6">
+        <f t="shared" si="0"/>
+        <v>-1.1755705045848952</v>
+      </c>
+    </row>
+    <row r="67" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B67" s="1">
         <f>(A67-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K67" s="1">
+        <v>2.9000000000000101</v>
+      </c>
+      <c r="L67" s="6">
+        <f t="shared" si="0"/>
+        <v>-0.61803398874983495</v>
+      </c>
+    </row>
+    <row r="68" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B68" s="1">
         <f>(A68-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K68" s="1">
+        <v>3.0000000000000102</v>
+      </c>
+      <c r="L68" s="6">
+        <f t="shared" si="0"/>
+        <v>6.2968727454482121E-14</v>
+      </c>
+    </row>
+    <row r="69" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B69" s="1">
         <f>(A69-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K69" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="L69" s="6">
+        <f t="shared" si="0"/>
+        <v>0.6180339887498939</v>
+      </c>
+    </row>
+    <row r="70" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B70" s="1">
         <f>(A70-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K70" s="1">
+        <v>3.2000000000000099</v>
+      </c>
+      <c r="L70" s="6">
+        <f t="shared" si="0"/>
+        <v>1.1755705045849971</v>
+      </c>
+    </row>
+    <row r="71" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B71" s="1">
         <f>(A71-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K71" s="1">
+        <v>3.30000000000001</v>
+      </c>
+      <c r="L71" s="6">
+        <f t="shared" si="0"/>
+        <v>1.6180339887499318</v>
+      </c>
+    </row>
+    <row r="72" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B72" s="1">
         <f>(A72-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K72" s="1">
+        <v>3.4000000000000101</v>
+      </c>
+      <c r="L72" s="6">
+        <f t="shared" si="0"/>
+        <v>1.9021130325903266</v>
+      </c>
+    </row>
+    <row r="73" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B73" s="1">
         <f>(A73-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K73" s="1">
+        <v>3.5000000000000102</v>
+      </c>
+      <c r="L73" s="6">
+        <f t="shared" ref="L73:L136" si="3">$H$7*SIN(($H$8*K73)-$H$9)+$H$11</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B74" s="1">
         <f>(A74-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K74" s="1">
+        <v>3.6000000000000099</v>
+      </c>
+      <c r="L74" s="6">
+        <f t="shared" si="3"/>
+        <v>1.9021130325902889</v>
+      </c>
+    </row>
+    <row r="75" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B75" s="1">
         <f>(A75-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K75" s="1">
+        <v>3.7000000000000099</v>
+      </c>
+      <c r="L75" s="6">
+        <f t="shared" si="3"/>
+        <v>1.618033988749858</v>
+      </c>
+    </row>
+    <row r="76" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B76" s="1">
         <f>(A76-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K76" s="1">
+        <v>3.80000000000001</v>
+      </c>
+      <c r="L76" s="6">
+        <f t="shared" si="3"/>
+        <v>1.1755705045848954</v>
+      </c>
+    </row>
+    <row r="77" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B77" s="1">
         <f>(A77-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K77" s="1">
+        <v>3.9000000000000101</v>
+      </c>
+      <c r="L77" s="6">
+        <f t="shared" si="3"/>
+        <v>0.61803398874983517</v>
+      </c>
+    </row>
+    <row r="78" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B78" s="1">
         <f>(A78-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K78" s="1">
+        <v>4.0000000000000098</v>
+      </c>
+      <c r="L78" s="6">
+        <f t="shared" si="3"/>
+        <v>-5.9170984084699896E-14</v>
+      </c>
+    </row>
+    <row r="79" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B79" s="1">
         <f>(A79-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K79" s="1">
+        <v>4.1000000000000103</v>
+      </c>
+      <c r="L79" s="6">
+        <f t="shared" si="3"/>
+        <v>-0.61803398874995785</v>
+      </c>
+    </row>
+    <row r="80" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B80" s="1">
         <f>(A80-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K80" s="1">
+        <v>4.2000000000000099</v>
+      </c>
+      <c r="L80" s="6">
+        <f t="shared" si="3"/>
+        <v>-1.1755705045849969</v>
+      </c>
+    </row>
+    <row r="81" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B81" s="1">
         <f>(A81-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K81" s="1">
+        <v>4.3000000000000096</v>
+      </c>
+      <c r="L81" s="6">
+        <f t="shared" si="3"/>
+        <v>-1.6180339887499295</v>
+      </c>
+    </row>
+    <row r="82" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B82" s="1">
         <f>(A82-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K82" s="1">
+        <v>4.4000000000000101</v>
+      </c>
+      <c r="L82" s="6">
+        <f t="shared" si="3"/>
+        <v>-1.9021130325903266</v>
+      </c>
+    </row>
+    <row r="83" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B83" s="1">
         <f>(A83-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K83" s="1">
+        <v>4.5000000000000098</v>
+      </c>
+      <c r="L83" s="6">
+        <f t="shared" si="3"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="84" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B84" s="1">
         <f>(A84-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K84" s="1">
+        <v>4.6000000000000103</v>
+      </c>
+      <c r="L84" s="6">
+        <f t="shared" si="3"/>
+        <v>-1.9021130325902877</v>
+      </c>
+    </row>
+    <row r="85" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B85" s="1">
         <f>(A85-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K85" s="1">
+        <v>4.7000000000000099</v>
+      </c>
+      <c r="L85" s="6">
+        <f t="shared" si="3"/>
+        <v>-1.6180339887498603</v>
+      </c>
+    </row>
+    <row r="86" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B86" s="1">
         <f>(A86-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K86" s="1">
+        <v>4.8000000000000096</v>
+      </c>
+      <c r="L86" s="6">
+        <f t="shared" si="3"/>
+        <v>-1.1755705045848956</v>
+      </c>
+    </row>
+    <row r="87" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B87" s="1">
         <f>(A87-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K87" s="1">
+        <v>4.9000000000000101</v>
+      </c>
+      <c r="L87" s="6">
+        <f t="shared" si="3"/>
+        <v>-0.61803398874983206</v>
+      </c>
+    </row>
+    <row r="88" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B88" s="1">
         <f>(A88-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K88" s="1">
+        <v>5.0000000000000098</v>
+      </c>
+      <c r="L88" s="6">
+        <f t="shared" si="3"/>
+        <v>5.5373240714917671E-14</v>
+      </c>
+    </row>
+    <row r="89" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B89" s="1">
         <f>(A89-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K89" s="1">
+        <v>5.1000000000000103</v>
+      </c>
+      <c r="L89" s="6">
+        <f t="shared" si="3"/>
+        <v>0.61803398874995763</v>
+      </c>
+    </row>
+    <row r="90" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B90" s="1">
         <f>(A90-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K90" s="1">
+        <v>5.2000000000000099</v>
+      </c>
+      <c r="L90" s="6">
+        <f t="shared" si="3"/>
+        <v>1.1755705045849967</v>
+      </c>
+    </row>
+    <row r="91" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B91" s="1">
         <f>(A91-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K91" s="1">
+        <v>5.3000000000000096</v>
+      </c>
+      <c r="L91" s="6">
+        <f t="shared" si="3"/>
+        <v>1.6180339887499295</v>
+      </c>
+    </row>
+    <row r="92" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B92" s="1">
         <f>(A92-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K92" s="1">
+        <v>5.4000000000000101</v>
+      </c>
+      <c r="L92" s="6">
+        <f t="shared" si="3"/>
+        <v>1.9021130325903264</v>
+      </c>
+    </row>
+    <row r="93" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B93" s="1">
         <f>(A93-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K93" s="1">
+        <v>5.5000000000000098</v>
+      </c>
+      <c r="L93" s="6">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B94" s="1">
         <f>(A94-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K94" s="1">
+        <v>5.6000000000000103</v>
+      </c>
+      <c r="L94" s="6">
+        <f t="shared" si="3"/>
+        <v>1.902113032590288</v>
+      </c>
+    </row>
+    <row r="95" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B95" s="1">
         <f>(A95-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K95" s="1">
+        <v>5.7000000000000099</v>
+      </c>
+      <c r="L95" s="6">
+        <f t="shared" si="3"/>
+        <v>1.6180339887498603</v>
+      </c>
+    </row>
+    <row r="96" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B96" s="1">
         <f>(A96-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K96" s="1">
+        <v>5.8000000000000096</v>
+      </c>
+      <c r="L96" s="6">
+        <f t="shared" si="3"/>
+        <v>1.1755705045849016</v>
+      </c>
+    </row>
+    <row r="97" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B97" s="1">
         <f>(A97-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K97" s="1">
+        <v>5.9000000000000101</v>
+      </c>
+      <c r="L97" s="6">
+        <f t="shared" si="3"/>
+        <v>0.61803398874983906</v>
+      </c>
+    </row>
+    <row r="98" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B98" s="1">
         <f>(A98-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K98" s="1">
+        <v>6.0000000000000098</v>
+      </c>
+      <c r="L98" s="6">
+        <f t="shared" si="3"/>
+        <v>-6.2233638381536949E-14</v>
+      </c>
+    </row>
+    <row r="99" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B99" s="1">
         <f>(A99-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K99" s="1">
+        <v>6.1000000000000103</v>
+      </c>
+      <c r="L99" s="6">
+        <f t="shared" si="3"/>
+        <v>-0.61803398874995741</v>
+      </c>
+    </row>
+    <row r="100" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B100" s="1">
         <f>(A100-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K100" s="1">
+        <v>6.2000000000000099</v>
+      </c>
+      <c r="L100" s="6">
+        <f t="shared" si="3"/>
+        <v>-1.1755705045849965</v>
+      </c>
+    </row>
+    <row r="101" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B101" s="1">
         <f>(A101-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K101" s="1">
+        <v>6.3000000000000096</v>
+      </c>
+      <c r="L101" s="6">
+        <f t="shared" si="3"/>
+        <v>-1.6180339887499293</v>
+      </c>
+    </row>
+    <row r="102" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B102" s="1">
         <f>(A102-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K102" s="1">
+        <v>6.4000000000000101</v>
+      </c>
+      <c r="L102" s="6">
+        <f t="shared" si="3"/>
+        <v>-1.9021130325903264</v>
+      </c>
+    </row>
+    <row r="103" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B103" s="1">
         <f>(A103-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K103" s="1">
+        <v>6.5000000000000098</v>
+      </c>
+      <c r="L103" s="6">
+        <f t="shared" si="3"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="104" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B104" s="1">
         <f>(A104-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K104" s="1">
+        <v>6.6000000000000103</v>
+      </c>
+      <c r="L104" s="6">
+        <f t="shared" si="3"/>
+        <v>-1.902113032590288</v>
+      </c>
+    </row>
+    <row r="105" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B105" s="1">
         <f>(A105-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K105" s="1">
+        <v>6.7000000000000099</v>
+      </c>
+      <c r="L105" s="6">
+        <f t="shared" si="3"/>
+        <v>-1.6180339887498605</v>
+      </c>
+    </row>
+    <row r="106" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B106" s="1">
         <f>(A106-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K106" s="1">
+        <v>6.8000000000000096</v>
+      </c>
+      <c r="L106" s="6">
+        <f t="shared" si="3"/>
+        <v>-1.1755705045849019</v>
+      </c>
+    </row>
+    <row r="107" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B107" s="1">
         <f>(A107-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K107" s="1">
+        <v>6.9000000000000101</v>
+      </c>
+      <c r="L107" s="6">
+        <f t="shared" si="3"/>
+        <v>-0.61803398874983928</v>
+      </c>
+    </row>
+    <row r="108" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B108" s="1">
         <f>(A108-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K108" s="1">
+        <v>7</v>
+      </c>
+      <c r="L108" s="6">
+        <f t="shared" si="3"/>
+        <v>-1.960237527853792E-15</v>
+      </c>
+    </row>
+    <row r="109" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B109" s="1">
         <f>(A109-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K109" s="1">
+        <v>7.1</v>
+      </c>
+      <c r="L109" s="6">
+        <f t="shared" si="3"/>
+        <v>0.61803398874988957</v>
+      </c>
+    </row>
+    <row r="110" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B110" s="1">
         <f>(A110-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K110" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="L110" s="6">
+        <f t="shared" si="3"/>
+        <v>1.1755705045849447</v>
+      </c>
+    </row>
+    <row r="111" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B111" s="1">
         <f>(A111-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K111" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="L111" s="6">
+        <f t="shared" si="3"/>
+        <v>1.6180339887498916</v>
+      </c>
+    </row>
+    <row r="112" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B112" s="1">
         <f>(A112-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K112" s="1">
+        <v>7.4</v>
+      </c>
+      <c r="L112" s="6">
+        <f t="shared" si="3"/>
+        <v>1.9021130325903066</v>
+      </c>
+    </row>
+    <row r="113" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B113" s="1">
         <f>(A113-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K113" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="L113" s="6">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B114" s="1">
         <f>(A114-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K114" s="1">
+        <v>7.6</v>
+      </c>
+      <c r="L114" s="6">
+        <f t="shared" si="3"/>
+        <v>1.9021130325903077</v>
+      </c>
+    </row>
+    <row r="115" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B115" s="1">
         <f>(A115-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K115" s="1">
+        <v>7.7</v>
+      </c>
+      <c r="L115" s="6">
+        <f t="shared" si="3"/>
+        <v>1.618033988749894</v>
+      </c>
+    </row>
+    <row r="116" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B116" s="1">
         <f>(A116-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K116" s="1">
+        <v>7.8</v>
+      </c>
+      <c r="L116" s="6">
+        <f t="shared" si="3"/>
+        <v>1.1755705045849481</v>
+      </c>
+    </row>
+    <row r="117" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B117" s="1">
         <f>(A117-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K117" s="1">
+        <v>7.9</v>
+      </c>
+      <c r="L117" s="6">
+        <f t="shared" si="3"/>
+        <v>0.61803398874989357</v>
+      </c>
+    </row>
+    <row r="118" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B118" s="1">
         <f>(A118-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K118" s="1">
+        <v>8</v>
+      </c>
+      <c r="L118" s="6">
+        <f t="shared" si="3"/>
+        <v>2.205267218835516E-15</v>
+      </c>
+    </row>
+    <row r="119" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B119" s="1">
         <f>(A119-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K119" s="1">
+        <v>8.1</v>
+      </c>
+      <c r="L119" s="6">
+        <f t="shared" si="3"/>
+        <v>-0.61803398874988935</v>
+      </c>
+    </row>
+    <row r="120" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B120" s="1">
         <f>(A120-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K120" s="1">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="L120" s="6">
+        <f t="shared" si="3"/>
+        <v>-1.1755705045849387</v>
+      </c>
+    </row>
+    <row r="121" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B121" s="1">
         <f>(A121-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K121" s="1">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="L121" s="6">
+        <f t="shared" si="3"/>
+        <v>-1.6180339887498956</v>
+      </c>
+    </row>
+    <row r="122" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B122" s="1">
         <f>(A122-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K122" s="1">
+        <v>8.4</v>
+      </c>
+      <c r="L122" s="6">
+        <f t="shared" si="3"/>
+        <v>-1.9021130325903064</v>
+      </c>
+    </row>
+    <row r="123" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B123" s="1">
         <f>(A123-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K123" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="L123" s="6">
+        <f t="shared" si="3"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="124" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B124" s="1">
         <f>(A124-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K124" s="1">
+        <v>8.6</v>
+      </c>
+      <c r="L124" s="6">
+        <f t="shared" si="3"/>
+        <v>-1.902113032590308</v>
+      </c>
+    </row>
+    <row r="125" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B125" s="1">
         <f>(A125-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K125" s="1">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="L125" s="6">
+        <f t="shared" si="3"/>
+        <v>-1.6180339887498982</v>
+      </c>
+    </row>
+    <row r="126" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B126" s="1">
         <f>(A126-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K126" s="1">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="L126" s="6">
+        <f t="shared" si="3"/>
+        <v>-1.1755705045849425</v>
+      </c>
+    </row>
+    <row r="127" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B127" s="1">
         <f>(A127-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K127" s="1">
+        <v>8.9</v>
+      </c>
+      <c r="L127" s="6">
+        <f t="shared" si="3"/>
+        <v>-0.61803398874989379</v>
+      </c>
+    </row>
+    <row r="128" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B128" s="1">
         <f>(A128-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K128" s="1">
+        <v>9</v>
+      </c>
+      <c r="L128" s="6">
+        <f t="shared" si="3"/>
+        <v>-2.45029690981724E-15</v>
+      </c>
+    </row>
+    <row r="129" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B129" s="1">
         <f>(A129-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K129" s="1">
+        <v>9.1</v>
+      </c>
+      <c r="L129" s="6">
+        <f t="shared" si="3"/>
+        <v>0.61803398874988913</v>
+      </c>
+    </row>
+    <row r="130" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B130" s="1">
         <f>(A130-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K130" s="1">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="L130" s="6">
+        <f t="shared" si="3"/>
+        <v>1.1755705045849385</v>
+      </c>
+    </row>
+    <row r="131" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B131" s="1">
         <f>(A131-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K131" s="1">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="L131" s="6">
+        <f t="shared" si="3"/>
+        <v>1.6180339887498913</v>
+      </c>
+    </row>
+    <row r="132" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B132" s="1">
         <f>(A132-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K132" s="1">
+        <v>9.4</v>
+      </c>
+      <c r="L132" s="6">
+        <f t="shared" si="3"/>
+        <v>1.9021130325903064</v>
+      </c>
+    </row>
+    <row r="133" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B133" s="1">
         <f>(A133-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K133" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="L133" s="6">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B134" s="1">
         <f>(A134-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K134" s="1">
+        <v>9.6</v>
+      </c>
+      <c r="L134" s="6">
+        <f t="shared" si="3"/>
+        <v>1.9021130325903057</v>
+      </c>
+    </row>
+    <row r="135" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B135" s="1">
         <f>(A135-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K135" s="1">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="L135" s="6">
+        <f t="shared" si="3"/>
+        <v>1.6180339887498985</v>
+      </c>
+    </row>
+    <row r="136" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B136" s="1">
         <f>(A136-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K136" s="1">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="L136" s="6">
+        <f t="shared" si="3"/>
+        <v>1.1755705045849369</v>
+      </c>
+    </row>
+    <row r="137" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B137" s="1">
         <f>(A137-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K137" s="1">
+        <v>9.9</v>
+      </c>
+      <c r="L137" s="6">
+        <f t="shared" ref="L137:L138" si="4">$H$7*SIN(($H$8*K137)-$H$9)+$H$11</f>
+        <v>0.61803398874989401</v>
+      </c>
+    </row>
+    <row r="138" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B138" s="1">
         <f>(A138-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
-    </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="K138" s="1">
+        <v>10</v>
+      </c>
+      <c r="L138" s="6">
+        <f t="shared" si="4"/>
+        <v>9.8007539583999659E-15</v>
+      </c>
+    </row>
+    <row r="139" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B139" s="1">
         <f>(A139-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B140" s="1">
         <f>(A140-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B141" s="1">
         <f>(A141-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B142" s="1">
         <f>(A142-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
     </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B143" s="1">
         <f>(A143-$E$1)^2</f>
         <v>251422.01640000002</v>
       </c>
     </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B144" s="1">
         <f>(A144-$E$1)^2</f>
         <v>251422.01640000002</v>
@@ -6593,5 +9863,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>